<commit_message>
feat: add parameters to check box tests
</commit_message>
<xml_diff>
--- a/demoqacomTest/src/test/resources/testParametrs.xlsx
+++ b/demoqacomTest/src/test/resources/testParametrs.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepo\portfolio\demoqa.com.Tests\demoqa.com.Tests\demoqacomTest\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3688E87F-C14A-471B-A6EA-F5EE647AACA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0DF55D-32D0-4EA7-8A66-CAC012DB2705}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37485" yWindow="720" windowWidth="16215" windowHeight="14385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchBookPositive" sheetId="2" r:id="rId1"/>
     <sheet name="SearchAuthorNegative" sheetId="3" r:id="rId2"/>
     <sheet name="userPositive" sheetId="1" r:id="rId3"/>
+    <sheet name="CheckBox" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>login</t>
   </si>
@@ -57,6 +58,36 @@
   </si>
   <si>
     <t>0!-Ivanov</t>
+  </si>
+  <si>
+    <t>Box</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Desktop React</t>
+  </si>
+  <si>
+    <t>desktop notes commands react</t>
+  </si>
+  <si>
+    <t>Classified</t>
+  </si>
+  <si>
+    <t>classified</t>
+  </si>
+  <si>
+    <t>home desktop notes commands documents workspace react angular veu office public private classified general downloads wordFile excelFile</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Home WorkSpace Public</t>
+  </si>
+  <si>
+    <t>desktop notes commands private classified general downloads wordFile excelFile</t>
   </si>
 </sst>
 </file>
@@ -448,7 +479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -477,4 +508,62 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60D15E4A-BEA6-4E8E-93CA-B7265D153B19}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>